<commit_message>
edited readme and metadata sheet
</commit_message>
<xml_diff>
--- a/spreadsheet_info.xlsx
+++ b/spreadsheet_info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veggerk/Desktop/John Day reservoir iso data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veggerk/Desktop/projects/walleye/Columbia-River-predatory-fish-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F185877-A2BA-5642-A112-337829086FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB2FDFD-34A5-B94E-8E1F-285B2EAC52B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="500" windowWidth="28040" windowHeight="15820" xr2:uid="{79E93AB8-230D-314D-8755-9704E32E46DF}"/>
+    <workbookView xWindow="200" yWindow="500" windowWidth="28040" windowHeight="15820" activeTab="1" xr2:uid="{79E93AB8-230D-314D-8755-9704E32E46DF}"/>
   </bookViews>
   <sheets>
     <sheet name="clean data column names" sheetId="1" r:id="rId1"/>
@@ -90,12 +90,6 @@
     <t>the total length of the individual measured in millimeters</t>
   </si>
   <si>
-    <t xml:space="preserve">denotes whether the individual was smaller or larger than 500mm, this is only applicable for walleye, as they needed to be separated into distinct size classes for the model to run </t>
-  </si>
-  <si>
-    <t>the timing of sample collection relative to the juvenile salmonid outmigration</t>
-  </si>
-  <si>
     <t>the month the sample was collected</t>
   </si>
   <si>
@@ -108,12 +102,6 @@
     <t>the common name of the individual</t>
   </si>
   <si>
-    <t>the percent carbon of the sample, not used for this analysis</t>
-  </si>
-  <si>
-    <t>the percent nitrogen of the sample, not used for this analysis</t>
-  </si>
-  <si>
     <t>the nitrogen stable isotope ratio</t>
   </si>
   <si>
@@ -130,6 +118,18 @@
   </si>
   <si>
     <t>This stable isotope data was collected in March through September of 2012 in the Upper John Day Reservoir in Washington State, USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denotes whether the individual was smaller or larger than 500mm, this is only applicable for walleye, as they needed to be separated into distinct size classes for the size effect model to run </t>
+  </si>
+  <si>
+    <t>the timing of sample collection relative to the juvenile salmonid outmigration through the area</t>
+  </si>
+  <si>
+    <t>the percent nitrogen of the sample</t>
+  </si>
+  <si>
+    <t>the percent carbon of the sample</t>
   </si>
 </sst>
 </file>
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D3303C-49B2-384D-8AB6-F6D6E99E07F9}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -496,7 +496,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -517,7 +517,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -533,7 +533,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -541,7 +541,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -549,7 +549,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -557,7 +557,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -565,7 +565,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -573,7 +573,7 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -581,7 +581,7 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -589,7 +589,7 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -597,7 +597,7 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -605,7 +605,7 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BE27593-0D52-7546-969C-74D1FB7B64EA}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -639,7 +639,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -655,7 +655,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -663,7 +663,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -671,7 +671,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -679,7 +679,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -687,7 +687,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -695,7 +695,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -703,7 +703,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>